<commit_message>
tomo report reader v1
</commit_message>
<xml_diff>
--- a/Plancheck/check_protocol/STEC poumon DCA.xlsx
+++ b/Plancheck/check_protocol/STEC poumon DCA.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="5400" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="5400"/>
   </bookViews>
   <sheets>
     <sheet name="General data" sheetId="1" r:id="rId1"/>
@@ -523,7 +523,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1207,11 +1207,11 @@
     <cellStyle name="Avertissement" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Calcul" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Cellule liée" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Commentaire" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Entrée" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Insatisfaisant" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Neutre" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Satisfaisant" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Sortie" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Texte explicatif" xfId="16" builtinId="53" customBuiltin="1"/>
@@ -1504,8 +1504,8 @@
   </sheetPr>
   <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2331,7 +2331,7 @@
   </sheetPr>
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>

</xml_diff>